<commit_message>
Cleaning up unused files
</commit_message>
<xml_diff>
--- a/ModalityLexiconSubcatTagsPITT.xlsx
+++ b/ModalityLexiconSubcatTagsPITT.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miszVPgbH+yhC6xsocpol/UWVDHVA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miu/0sgByzQzgEnB3yOWb7nfpRl0A=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="234">
   <si>
     <t>Lexical item</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>presuppose</t>
+  </si>
+  <si>
+    <t>probably</t>
   </si>
   <si>
     <t>suppose</t>
@@ -1916,16 +1919,16 @@
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="6">
         <v>2.0</v>
       </c>
     </row>
@@ -1958,55 +1961,55 @@
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="22" t="s">
+      <c r="B44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="23">
-        <v>2.0</v>
-      </c>
-      <c r="G44" s="24"/>
-      <c r="I44" s="25" t="s">
+      <c r="F44" s="5">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="26"/>
-      <c r="M44" s="26"/>
-      <c r="N44" s="26"/>
-      <c r="O44" s="26"/>
-      <c r="P44" s="26"/>
-      <c r="Q44" s="26"/>
-      <c r="R44" s="26"/>
-      <c r="S44" s="26"/>
-      <c r="T44" s="26"/>
-      <c r="U44" s="26"/>
-      <c r="V44" s="26"/>
-      <c r="W44" s="26"/>
-      <c r="X44" s="26"/>
-      <c r="Y44" s="26"/>
-      <c r="Z44" s="10"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="5" t="s">
+      <c r="B45" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="23">
+        <v>2.0</v>
+      </c>
+      <c r="G45" s="24"/>
+      <c r="I45" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="5">
-        <v>2.0</v>
-      </c>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+      <c r="R45" s="26"/>
+      <c r="S45" s="26"/>
+      <c r="T45" s="26"/>
+      <c r="U45" s="26"/>
+      <c r="V45" s="26"/>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
+      <c r="Y45" s="26"/>
+      <c r="Z45" s="10"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="5" t="s">
@@ -2016,27 +2019,21 @@
         <v>21</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="F46" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="G46" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>48</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="F47" s="5">
         <v>1.0</v>
@@ -2056,10 +2053,16 @@
         <v>21</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F48" s="5">
         <v>1.0</v>
+      </c>
+      <c r="G48" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
@@ -2070,73 +2073,73 @@
         <v>21</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F49" s="5">
         <v>1.0</v>
       </c>
-      <c r="G49" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B50" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F50" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="G50" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="H50" s="8" t="b">
+      <c r="B50" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="G50" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="28"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="G51" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="H51" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="I50" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="26"/>
-      <c r="N50" s="26"/>
-      <c r="O50" s="26"/>
-      <c r="P50" s="26"/>
-      <c r="Q50" s="26"/>
-      <c r="R50" s="26"/>
-      <c r="S50" s="26"/>
-      <c r="T50" s="26"/>
-      <c r="U50" s="26"/>
-      <c r="V50" s="26"/>
-      <c r="W50" s="26"/>
-      <c r="X50" s="26"/>
-      <c r="Y50" s="26"/>
-      <c r="Z50" s="10"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="5" t="s">
+      <c r="I51" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F51" s="5">
-        <v>1.0</v>
-      </c>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
+      <c r="P51" s="26"/>
+      <c r="Q51" s="26"/>
+      <c r="R51" s="26"/>
+      <c r="S51" s="26"/>
+      <c r="T51" s="26"/>
+      <c r="U51" s="26"/>
+      <c r="V51" s="26"/>
+      <c r="W51" s="26"/>
+      <c r="X51" s="26"/>
+      <c r="Y51" s="26"/>
+      <c r="Z51" s="10"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="5" t="s">
@@ -2146,7 +2149,7 @@
         <v>21</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F52" s="5">
         <v>1.0</v>
@@ -2160,56 +2163,50 @@
         <v>21</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F53" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="F54" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="G54" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="H54" s="27"/>
-      <c r="I54" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="J54" s="31" t="s">
+      <c r="B54" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F54" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="31" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="5" t="s">
+      <c r="B55" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F55" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="G55" s="31">
+        <v>1.0</v>
+      </c>
+      <c r="H55" s="27"/>
+      <c r="I55" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="J55" s="31" t="s">
         <v>88</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F55" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="G55" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I55" s="12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
@@ -2220,10 +2217,16 @@
         <v>21</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F56" s="5">
         <v>1.0</v>
+      </c>
+      <c r="G56" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
@@ -2234,16 +2237,10 @@
         <v>21</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F57" s="5">
         <v>1.0</v>
-      </c>
-      <c r="G57" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I57" s="12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
@@ -2254,7 +2251,7 @@
         <v>21</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F58" s="5">
         <v>1.0</v>
@@ -2274,7 +2271,7 @@
         <v>21</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F59" s="5">
         <v>1.0</v>
@@ -2294,7 +2291,7 @@
         <v>21</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F60" s="5">
         <v>1.0</v>
@@ -2314,10 +2311,16 @@
         <v>21</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F61" s="5">
         <v>1.0</v>
+      </c>
+      <c r="G61" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
@@ -2328,16 +2331,10 @@
         <v>21</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F62" s="5">
         <v>1.0</v>
-      </c>
-      <c r="G62" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I62" s="12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
@@ -2348,10 +2345,10 @@
         <v>21</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F63" s="8">
-        <v>2.0</v>
+        <v>78</v>
+      </c>
+      <c r="F63" s="5">
+        <v>1.0</v>
       </c>
       <c r="G63" s="12">
         <v>1.0</v>
@@ -2362,16 +2359,22 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F64" s="5">
-        <v>3.0</v>
+      <c r="F64" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="G64" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
@@ -2382,7 +2385,7 @@
         <v>21</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F65" s="5">
         <v>3.0</v>
@@ -2396,7 +2399,7 @@
         <v>21</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F66" s="5">
         <v>3.0</v>
@@ -2404,36 +2407,36 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="5" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F67" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="G67" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I67" s="12" t="s">
-        <v>48</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="F68" s="5">
         <v>2.0</v>
+      </c>
+      <c r="G68" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I68" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
@@ -2444,7 +2447,7 @@
         <v>21</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F69" s="5">
         <v>2.0</v>
@@ -2458,7 +2461,7 @@
         <v>21</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F70" s="5">
         <v>2.0</v>
@@ -2472,7 +2475,7 @@
         <v>21</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F71" s="5">
         <v>2.0</v>
@@ -2486,7 +2489,7 @@
         <v>21</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F72" s="5">
         <v>2.0</v>
@@ -2500,7 +2503,7 @@
         <v>21</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F73" s="5">
         <v>2.0</v>
@@ -2514,16 +2517,10 @@
         <v>21</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F74" s="5">
         <v>2.0</v>
-      </c>
-      <c r="G74" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I74" s="12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
@@ -2534,10 +2531,16 @@
         <v>21</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F75" s="5">
         <v>2.0</v>
+      </c>
+      <c r="G75" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I75" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
@@ -2548,7 +2551,7 @@
         <v>21</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F76" s="5">
         <v>2.0</v>
@@ -2562,7 +2565,7 @@
         <v>21</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F77" s="5">
         <v>2.0</v>
@@ -2576,7 +2579,7 @@
         <v>21</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F78" s="5">
         <v>2.0</v>
@@ -2590,7 +2593,7 @@
         <v>21</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F79" s="5">
         <v>2.0</v>
@@ -2604,7 +2607,7 @@
         <v>21</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F80" s="5">
         <v>2.0</v>
@@ -2618,7 +2621,7 @@
         <v>21</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F81" s="5">
         <v>2.0</v>
@@ -2632,7 +2635,7 @@
         <v>21</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F82" s="5">
         <v>2.0</v>
@@ -2640,50 +2643,47 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="5" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F83" s="5">
         <v>2.0</v>
-      </c>
-      <c r="G83" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I83" s="12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="5" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>118</v>
+        <v>21</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="F84" s="5">
-        <v>-3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G84" s="12">
-        <v>-1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="I84" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="F85" s="5">
         <v>-3.0</v>
@@ -2697,10 +2697,10 @@
         <v>121</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F86" s="5">
         <v>-3.0</v>
@@ -2714,19 +2714,16 @@
         <v>122</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F87" s="5">
         <v>-3.0</v>
       </c>
       <c r="G87" s="12">
         <v>-1.0</v>
-      </c>
-      <c r="H87" s="5" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
@@ -2734,38 +2731,44 @@
         <v>123</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F88" s="5">
-        <v>-2.0</v>
+        <v>-3.0</v>
+      </c>
+      <c r="G88" s="12">
+        <v>-1.0</v>
+      </c>
+      <c r="H88" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B89" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="F89" s="5">
-        <v>-3.0</v>
+        <v>-2.0</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="F90" s="5">
         <v>-3.0</v>
@@ -2779,27 +2782,21 @@
         <v>21</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F91" s="5">
         <v>-3.0</v>
       </c>
-      <c r="G91" s="32">
-        <v>-1.0</v>
-      </c>
-      <c r="I91" s="33" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F92" s="5">
         <v>-3.0</v>
@@ -2808,7 +2805,7 @@
         <v>-1.0</v>
       </c>
       <c r="I92" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
@@ -2819,7 +2816,7 @@
         <v>21</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F93" s="5">
         <v>-3.0</v>
@@ -2828,139 +2825,139 @@
         <v>-1.0</v>
       </c>
       <c r="I93" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E94" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F94" s="8">
+      <c r="E94" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F94" s="5">
         <v>-3.0</v>
       </c>
-      <c r="G94" s="12">
+      <c r="G94" s="32">
         <v>-1.0</v>
       </c>
-      <c r="I94" s="12" t="s">
+      <c r="I94" s="33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="95" ht="15.75" customHeight="1">
+      <c r="A95" s="8" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="5" t="s">
+      <c r="B95" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F95" s="8">
+        <v>-3.0</v>
+      </c>
+      <c r="G95" s="12">
+        <v>-1.0</v>
+      </c>
+      <c r="I95" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="B95" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E95" s="5" t="s">
+    </row>
+    <row r="96" ht="15.75" customHeight="1">
+      <c r="A96" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F95" s="5">
+      <c r="B96" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F96" s="5">
         <v>-2.0</v>
       </c>
-      <c r="G95" s="32">
+      <c r="G96" s="32">
         <v>-1.0</v>
       </c>
-      <c r="H95" s="8" t="b">
+      <c r="H96" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="I95" s="33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="27" t="s">
+      <c r="I96" s="33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="97" ht="15.75" customHeight="1">
+      <c r="A97" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B97" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B96" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="F96" s="27">
+      <c r="F97" s="27">
         <v>-2.0</v>
       </c>
-      <c r="G96" s="34">
+      <c r="G97" s="34">
         <v>-1.0</v>
       </c>
-      <c r="H96" s="27"/>
-      <c r="I96" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="J96" s="31" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="5" t="s">
+      <c r="H97" s="27"/>
+      <c r="I97" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="J97" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="B97" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F97" s="5">
-        <v>-2.0</v>
-      </c>
-      <c r="G97" s="32">
-        <v>-1.0</v>
-      </c>
-      <c r="I97" s="33" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="8" t="s">
+      <c r="A98" s="5" t="s">
         <v>139</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E98" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F98" s="8">
+      <c r="E98" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F98" s="5">
         <v>-2.0</v>
       </c>
       <c r="G98" s="32">
         <v>-1.0</v>
       </c>
-      <c r="H98" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="I98" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="8" t="s">
         <v>140</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E99" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F99" s="5">
+      <c r="E99" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F99" s="8">
         <v>-2.0</v>
       </c>
       <c r="G99" s="32">
         <v>-1.0</v>
       </c>
+      <c r="H99" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="I99" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
@@ -2971,7 +2968,7 @@
         <v>21</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F100" s="5">
         <v>-2.0</v>
@@ -2980,7 +2977,7 @@
         <v>-1.0</v>
       </c>
       <c r="I100" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
@@ -2991,7 +2988,7 @@
         <v>21</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F101" s="5">
         <v>-2.0</v>
@@ -3000,18 +2997,18 @@
         <v>-1.0</v>
       </c>
       <c r="I101" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E102" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="F102" s="5">
         <v>-2.0</v>
@@ -3020,7 +3017,7 @@
         <v>-1.0</v>
       </c>
       <c r="I102" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
@@ -3031,7 +3028,7 @@
         <v>21</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F103" s="5">
         <v>-2.0</v>
@@ -3040,76 +3037,76 @@
         <v>-1.0</v>
       </c>
       <c r="I103" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="27" t="s">
+      <c r="A104" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B104" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="F104" s="27">
+      <c r="B104" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F104" s="5">
         <v>-2.0</v>
       </c>
-      <c r="G104" s="34">
+      <c r="G104" s="32">
         <v>-1.0</v>
       </c>
-      <c r="H104" s="27"/>
-      <c r="I104" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="J104" s="31" t="s">
-        <v>87</v>
+      <c r="I104" s="33" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="F105" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="G105" s="12">
+      <c r="A105" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B105" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C105" s="27"/>
+      <c r="D105" s="27"/>
+      <c r="E105" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="F105" s="27">
+        <v>-2.0</v>
+      </c>
+      <c r="G105" s="34">
         <v>-1.0</v>
       </c>
-      <c r="H105" s="8" t="b">
+      <c r="H105" s="27"/>
+      <c r="I105" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="J105" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="106" ht="15.75" customHeight="1">
+      <c r="A106" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F106" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="G106" s="12">
+        <v>-1.0</v>
+      </c>
+      <c r="H106" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="I105" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F106" s="5">
-        <v>-2.0</v>
-      </c>
-      <c r="G106" s="32">
-        <v>-1.0</v>
-      </c>
-      <c r="I106" s="33" t="s">
-        <v>129</v>
+      <c r="I106" s="12" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
@@ -3120,7 +3117,7 @@
         <v>21</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F107" s="5">
         <v>-2.0</v>
@@ -3129,7 +3126,7 @@
         <v>-1.0</v>
       </c>
       <c r="I107" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
@@ -3140,27 +3137,27 @@
         <v>21</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F108" s="5">
-        <v>-3.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G108" s="32">
         <v>-1.0</v>
       </c>
       <c r="I108" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E109" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="F109" s="5">
         <v>-3.0</v>
@@ -3169,7 +3166,7 @@
         <v>-1.0</v>
       </c>
       <c r="I109" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
@@ -3180,7 +3177,7 @@
         <v>21</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F110" s="5">
         <v>-3.0</v>
@@ -3189,7 +3186,7 @@
         <v>-1.0</v>
       </c>
       <c r="I110" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
@@ -3197,10 +3194,10 @@
         <v>153</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F111" s="5">
         <v>-3.0</v>
@@ -3209,7 +3206,7 @@
         <v>-1.0</v>
       </c>
       <c r="I111" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
@@ -3220,7 +3217,7 @@
         <v>9</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F112" s="5">
         <v>-3.0</v>
@@ -3229,41 +3226,38 @@
         <v>-1.0</v>
       </c>
       <c r="I112" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="8" t="s">
+      <c r="A113" s="5" t="s">
         <v>155</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F113" s="8">
-        <v>-2.0</v>
-      </c>
-      <c r="G113" s="12">
+        <v>151</v>
+      </c>
+      <c r="F113" s="5">
+        <v>-3.0</v>
+      </c>
+      <c r="G113" s="32">
         <v>-1.0</v>
       </c>
-      <c r="H113" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I113" s="12" t="s">
-        <v>129</v>
+      <c r="I113" s="33" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E114" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="F114" s="8">
         <v>-2.0</v>
@@ -3275,70 +3269,73 @@
         <v>1</v>
       </c>
       <c r="I114" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="8" t="s">
         <v>158</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F115" s="5">
+        <v>157</v>
+      </c>
+      <c r="F115" s="8">
         <v>-2.0</v>
       </c>
       <c r="G115" s="12">
         <v>-1.0</v>
       </c>
+      <c r="H115" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="I115" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="8" t="s">
+      <c r="A116" s="5" t="s">
         <v>159</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F116" s="8">
-        <v>-3.0</v>
+        <v>157</v>
+      </c>
+      <c r="F116" s="5">
+        <v>-2.0</v>
       </c>
       <c r="G116" s="12">
         <v>-1.0</v>
       </c>
-      <c r="H116" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="I116" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="8" t="s">
         <v>160</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F117" s="5">
-        <v>-2.0</v>
+        <v>157</v>
+      </c>
+      <c r="F117" s="8">
+        <v>-3.0</v>
       </c>
       <c r="G117" s="12">
         <v>-1.0</v>
       </c>
+      <c r="H117" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="I117" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
@@ -3349,7 +3346,7 @@
         <v>21</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F118" s="5">
         <v>-2.0</v>
@@ -3358,7 +3355,7 @@
         <v>-1.0</v>
       </c>
       <c r="I118" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
@@ -3369,19 +3366,16 @@
         <v>21</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F119" s="5">
-        <v>-3.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G119" s="12">
         <v>-1.0</v>
       </c>
-      <c r="H119" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="I119" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
@@ -3392,40 +3386,43 @@
         <v>21</v>
       </c>
       <c r="E120" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F120" s="5">
+        <v>-3.0</v>
+      </c>
+      <c r="G120" s="12">
+        <v>-1.0</v>
+      </c>
+      <c r="H120" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I120" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="121" ht="15.75" customHeight="1">
+      <c r="A121" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F120" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="G120" s="12">
+      <c r="B121" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F121" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="G121" s="12">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H120" s="8" t="b">
+      <c r="H121" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="I120" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F121" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="G121" s="12">
-        <v>1.0</v>
-      </c>
       <c r="I121" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
@@ -3436,7 +3433,7 @@
         <v>21</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F122" s="5">
         <v>2.0</v>
@@ -3445,7 +3442,7 @@
         <v>1.0</v>
       </c>
       <c r="I122" s="12" t="s">
-        <v>48</v>
+        <v>130</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
@@ -3456,7 +3453,7 @@
         <v>21</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F123" s="5">
         <v>2.0</v>
@@ -3469,14 +3466,14 @@
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="8" t="s">
+      <c r="A124" s="5" t="s">
         <v>168</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F124" s="5">
         <v>2.0</v>
@@ -3489,14 +3486,14 @@
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="8" t="s">
         <v>169</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F125" s="5">
         <v>2.0</v>
@@ -3516,7 +3513,7 @@
         <v>21</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F126" s="5">
         <v>2.0</v>
@@ -3536,7 +3533,7 @@
         <v>21</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F127" s="5">
         <v>2.0</v>
@@ -3556,7 +3553,7 @@
         <v>21</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F128" s="5">
         <v>2.0</v>
@@ -3565,27 +3562,27 @@
         <v>1.0</v>
       </c>
       <c r="I128" s="12" t="s">
-        <v>173</v>
+        <v>48</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F129" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="G129" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I129" s="12" t="s">
         <v>174</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E129" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F129" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="G129" s="12">
-        <v>-1.0</v>
-      </c>
-      <c r="I129" s="12" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
@@ -3596,7 +3593,7 @@
         <v>21</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F130" s="5">
         <v>2.0</v>
@@ -3605,66 +3602,72 @@
         <v>-1.0</v>
       </c>
       <c r="I130" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="5" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F131" s="5">
         <v>2.0</v>
+      </c>
+      <c r="G131" s="12">
+        <v>-1.0</v>
+      </c>
+      <c r="I131" s="12" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E132" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B132" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E132" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="F132" s="5">
         <v>2.0</v>
-      </c>
-      <c r="G132" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="I132" s="36" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E133" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B133" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="E133" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="F133" s="5">
         <v>2.0</v>
+      </c>
+      <c r="G133" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="I133" s="36" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B134" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B134" s="5" t="s">
-        <v>180</v>
-      </c>
       <c r="E134" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F134" s="5">
         <v>2.0</v>
@@ -3672,13 +3675,13 @@
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B135" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B135" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="E135" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F135" s="5">
         <v>2.0</v>
@@ -3692,7 +3695,7 @@
         <v>21</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F136" s="5">
         <v>2.0</v>
@@ -3706,7 +3709,7 @@
         <v>21</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F137" s="5">
         <v>2.0</v>
@@ -3717,10 +3720,10 @@
         <v>184</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F138" s="5">
         <v>2.0</v>
@@ -3731,10 +3734,10 @@
         <v>185</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F139" s="5">
         <v>2.0</v>
@@ -3745,30 +3748,24 @@
         <v>186</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="F140" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="G140" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="I140" s="36" t="s">
-        <v>48</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E141" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E141" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="F141" s="5">
         <v>3.0</v>
@@ -3788,10 +3785,16 @@
         <v>21</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F142" s="5">
         <v>3.0</v>
+      </c>
+      <c r="G142" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="I142" s="36" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="143" ht="15.75" customHeight="1">
@@ -3802,7 +3805,7 @@
         <v>21</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F143" s="5">
         <v>3.0</v>
@@ -3816,16 +3819,10 @@
         <v>21</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F144" s="5">
         <v>3.0</v>
-      </c>
-      <c r="G144" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="I144" s="36" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1">
@@ -3836,7 +3833,7 @@
         <v>21</v>
       </c>
       <c r="E145" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F145" s="5">
         <v>3.0</v>
@@ -3856,10 +3853,16 @@
         <v>21</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F146" s="5">
         <v>3.0</v>
+      </c>
+      <c r="G146" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="I146" s="36" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1">
@@ -3870,7 +3873,7 @@
         <v>21</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F147" s="5">
         <v>3.0</v>
@@ -3884,16 +3887,10 @@
         <v>21</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F148" s="5">
         <v>3.0</v>
-      </c>
-      <c r="G148" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="I148" s="36" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="149" ht="15.75" customHeight="1">
@@ -3904,10 +3901,16 @@
         <v>21</v>
       </c>
       <c r="E149" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F149" s="5">
         <v>3.0</v>
+      </c>
+      <c r="G149" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="I149" s="36" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="150" ht="15.75" customHeight="1">
@@ -3918,16 +3921,10 @@
         <v>21</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F150" s="5">
         <v>3.0</v>
-      </c>
-      <c r="G150" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="I150" s="36" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="151" ht="15.75" customHeight="1">
@@ -3938,7 +3935,7 @@
         <v>21</v>
       </c>
       <c r="E151" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F151" s="5">
         <v>3.0</v>
@@ -3951,33 +3948,34 @@
       </c>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="8" t="s">
+      <c r="A152" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B152" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E152" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="F152" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="G152" s="8"/>
-      <c r="H152" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I152" s="8"/>
+      <c r="B152" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F152" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="G152" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="I152" s="36" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E153" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F153" s="8">
         <v>2.0</v>
@@ -3996,7 +3994,7 @@
         <v>14</v>
       </c>
       <c r="E154" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F154" s="8">
         <v>2.0</v>
@@ -4008,34 +4006,33 @@
       <c r="I154" s="8"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E155" s="5" t="s">
+      <c r="A155" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="F155" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="G155" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="I155" s="36" t="s">
-        <v>48</v>
-      </c>
+      <c r="B155" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E155" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F155" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="G155" s="8"/>
+      <c r="H155" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I155" s="8"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E156" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E156" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="F156" s="5">
         <v>2.0</v>
@@ -4055,7 +4052,7 @@
         <v>21</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F157" s="5">
         <v>2.0</v>
@@ -4074,37 +4071,18 @@
       <c r="B158" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E158" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="F158" s="12">
+      <c r="E158" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F158" s="5">
         <v>2.0</v>
       </c>
       <c r="G158" s="35">
         <v>1.0</v>
       </c>
-      <c r="H158" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="I158" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J158" s="10"/>
-      <c r="K158" s="10"/>
-      <c r="L158" s="10"/>
-      <c r="M158" s="10"/>
-      <c r="N158" s="10"/>
-      <c r="O158" s="10"/>
-      <c r="P158" s="10"/>
-      <c r="Q158" s="10"/>
-      <c r="R158" s="10"/>
-      <c r="S158" s="10"/>
-      <c r="T158" s="10"/>
-      <c r="U158" s="10"/>
-      <c r="V158" s="10"/>
-      <c r="W158" s="10"/>
-      <c r="X158" s="10"/>
-      <c r="Y158" s="10"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="5" t="s">
@@ -4114,7 +4092,7 @@
         <v>21</v>
       </c>
       <c r="E159" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F159" s="12">
         <v>2.0</v>
@@ -4153,7 +4131,7 @@
         <v>21</v>
       </c>
       <c r="E160" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F160" s="12">
         <v>2.0</v>
@@ -4192,7 +4170,7 @@
         <v>21</v>
       </c>
       <c r="E161" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F161" s="12">
         <v>2.0</v>
@@ -4230,18 +4208,37 @@
       <c r="B162" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E162" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F162" s="5">
+      <c r="E162" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="F162" s="12">
         <v>2.0</v>
       </c>
       <c r="G162" s="35">
         <v>1.0</v>
       </c>
+      <c r="H162" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="I162" s="36" t="s">
         <v>48</v>
       </c>
+      <c r="J162" s="10"/>
+      <c r="K162" s="10"/>
+      <c r="L162" s="10"/>
+      <c r="M162" s="10"/>
+      <c r="N162" s="10"/>
+      <c r="O162" s="10"/>
+      <c r="P162" s="10"/>
+      <c r="Q162" s="10"/>
+      <c r="R162" s="10"/>
+      <c r="S162" s="10"/>
+      <c r="T162" s="10"/>
+      <c r="U162" s="10"/>
+      <c r="V162" s="10"/>
+      <c r="W162" s="10"/>
+      <c r="X162" s="10"/>
+      <c r="Y162" s="10"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="5" t="s">
@@ -4251,7 +4248,7 @@
         <v>21</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F163" s="5">
         <v>2.0</v>
@@ -4264,14 +4261,14 @@
       </c>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="8" t="s">
+      <c r="A164" s="5" t="s">
         <v>212</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F164" s="5">
         <v>2.0</v>
@@ -4279,24 +4276,21 @@
       <c r="G164" s="35">
         <v>1.0</v>
       </c>
-      <c r="H164" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="I164" s="36" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="5" t="s">
+      <c r="A165" s="8" t="s">
         <v>213</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E165" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="F165" s="12">
+      <c r="E165" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F165" s="5">
         <v>2.0</v>
       </c>
       <c r="G165" s="35">
@@ -4308,34 +4302,18 @@
       <c r="I165" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J165" s="10"/>
-      <c r="K165" s="10"/>
-      <c r="L165" s="10"/>
-      <c r="M165" s="10"/>
-      <c r="N165" s="10"/>
-      <c r="O165" s="10"/>
-      <c r="P165" s="10"/>
-      <c r="Q165" s="10"/>
-      <c r="R165" s="10"/>
-      <c r="S165" s="10"/>
-      <c r="T165" s="10"/>
-      <c r="U165" s="10"/>
-      <c r="V165" s="10"/>
-      <c r="W165" s="10"/>
-      <c r="X165" s="10"/>
-      <c r="Y165" s="10"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="8" t="s">
+      <c r="A166" s="5" t="s">
         <v>214</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E166" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F166" s="5">
+      <c r="E166" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="F166" s="12">
         <v>2.0</v>
       </c>
       <c r="G166" s="35">
@@ -4347,22 +4325,41 @@
       <c r="I166" s="36" t="s">
         <v>48</v>
       </c>
+      <c r="J166" s="10"/>
+      <c r="K166" s="10"/>
+      <c r="L166" s="10"/>
+      <c r="M166" s="10"/>
+      <c r="N166" s="10"/>
+      <c r="O166" s="10"/>
+      <c r="P166" s="10"/>
+      <c r="Q166" s="10"/>
+      <c r="R166" s="10"/>
+      <c r="S166" s="10"/>
+      <c r="T166" s="10"/>
+      <c r="U166" s="10"/>
+      <c r="V166" s="10"/>
+      <c r="W166" s="10"/>
+      <c r="X166" s="10"/>
+      <c r="Y166" s="10"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="5" t="s">
+      <c r="A167" s="8" t="s">
         <v>215</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E167" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F167" s="5">
         <v>2.0</v>
       </c>
       <c r="G167" s="35">
         <v>1.0</v>
+      </c>
+      <c r="H167" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="I167" s="36" t="s">
         <v>48</v>
@@ -4376,7 +4373,7 @@
         <v>21</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F168" s="5">
         <v>2.0</v>
@@ -4396,7 +4393,7 @@
         <v>21</v>
       </c>
       <c r="E169" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F169" s="5">
         <v>2.0</v>
@@ -4416,7 +4413,7 @@
         <v>21</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F170" s="5">
         <v>2.0</v>
@@ -4424,22 +4421,19 @@
       <c r="G170" s="35">
         <v>1.0</v>
       </c>
-      <c r="H170" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I170" s="12" t="s">
+      <c r="I170" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="171" ht="15.75" customHeight="1">
+      <c r="A171" s="5" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="B171" s="37" t="s">
+      <c r="B171" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F171" s="5">
         <v>2.0</v>
@@ -4450,25 +4444,28 @@
       <c r="H171" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="I171" s="36" t="s">
-        <v>48</v>
+      <c r="I171" s="12" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="5" t="s">
+      <c r="A172" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="B172" s="37" t="s">
         <v>21</v>
       </c>
       <c r="E172" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F172" s="5">
         <v>2.0</v>
       </c>
       <c r="G172" s="35">
         <v>1.0</v>
+      </c>
+      <c r="H172" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="I172" s="36" t="s">
         <v>48</v>
@@ -4481,37 +4478,18 @@
       <c r="B173" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E173" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="F173" s="12">
-        <v>3.0</v>
+      <c r="E173" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F173" s="5">
+        <v>2.0</v>
       </c>
       <c r="G173" s="35">
         <v>1.0</v>
       </c>
-      <c r="H173" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="I173" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J173" s="10"/>
-      <c r="K173" s="10"/>
-      <c r="L173" s="10"/>
-      <c r="M173" s="10"/>
-      <c r="N173" s="10"/>
-      <c r="O173" s="10"/>
-      <c r="P173" s="10"/>
-      <c r="Q173" s="10"/>
-      <c r="R173" s="10"/>
-      <c r="S173" s="10"/>
-      <c r="T173" s="10"/>
-      <c r="U173" s="10"/>
-      <c r="V173" s="10"/>
-      <c r="W173" s="10"/>
-      <c r="X173" s="10"/>
-      <c r="Y173" s="10"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="5" t="s">
@@ -4520,28 +4498,47 @@
       <c r="B174" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E174" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F174" s="5">
-        <v>2.0</v>
+      <c r="E174" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="F174" s="12">
+        <v>3.0</v>
       </c>
       <c r="G174" s="35">
         <v>1.0</v>
       </c>
+      <c r="H174" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="I174" s="36" t="s">
         <v>48</v>
       </c>
+      <c r="J174" s="10"/>
+      <c r="K174" s="10"/>
+      <c r="L174" s="10"/>
+      <c r="M174" s="10"/>
+      <c r="N174" s="10"/>
+      <c r="O174" s="10"/>
+      <c r="P174" s="10"/>
+      <c r="Q174" s="10"/>
+      <c r="R174" s="10"/>
+      <c r="S174" s="10"/>
+      <c r="T174" s="10"/>
+      <c r="U174" s="10"/>
+      <c r="V174" s="10"/>
+      <c r="W174" s="10"/>
+      <c r="X174" s="10"/>
+      <c r="Y174" s="10"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="5" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E175" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F175" s="5">
         <v>2.0</v>
@@ -4555,13 +4552,13 @@
     </row>
     <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="5" t="s">
-        <v>224</v>
+        <v>178</v>
       </c>
       <c r="B176" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E176" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F176" s="5">
         <v>2.0</v>
@@ -4581,7 +4578,7 @@
         <v>21</v>
       </c>
       <c r="E177" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F177" s="5">
         <v>2.0</v>
@@ -4601,7 +4598,7 @@
         <v>21</v>
       </c>
       <c r="E178" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F178" s="5">
         <v>2.0</v>
@@ -4621,7 +4618,7 @@
         <v>21</v>
       </c>
       <c r="E179" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F179" s="5">
         <v>2.0</v>
@@ -4641,7 +4638,7 @@
         <v>21</v>
       </c>
       <c r="E180" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F180" s="5">
         <v>2.0</v>
@@ -4660,37 +4657,18 @@
       <c r="B181" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E181" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="F181" s="12">
-        <v>3.0</v>
+      <c r="E181" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F181" s="5">
+        <v>2.0</v>
       </c>
       <c r="G181" s="35">
         <v>1.0</v>
       </c>
-      <c r="H181" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="I181" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J181" s="10"/>
-      <c r="K181" s="10"/>
-      <c r="L181" s="10"/>
-      <c r="M181" s="10"/>
-      <c r="N181" s="10"/>
-      <c r="O181" s="10"/>
-      <c r="P181" s="10"/>
-      <c r="Q181" s="10"/>
-      <c r="R181" s="10"/>
-      <c r="S181" s="10"/>
-      <c r="T181" s="10"/>
-      <c r="U181" s="10"/>
-      <c r="V181" s="10"/>
-      <c r="W181" s="10"/>
-      <c r="X181" s="10"/>
-      <c r="Y181" s="10"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="5" t="s">
@@ -4699,18 +4677,37 @@
       <c r="B182" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E182" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F182" s="5">
-        <v>2.0</v>
+      <c r="E182" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="F182" s="12">
+        <v>3.0</v>
       </c>
       <c r="G182" s="35">
         <v>1.0</v>
       </c>
+      <c r="H182" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="I182" s="36" t="s">
         <v>48</v>
       </c>
+      <c r="J182" s="10"/>
+      <c r="K182" s="10"/>
+      <c r="L182" s="10"/>
+      <c r="M182" s="10"/>
+      <c r="N182" s="10"/>
+      <c r="O182" s="10"/>
+      <c r="P182" s="10"/>
+      <c r="Q182" s="10"/>
+      <c r="R182" s="10"/>
+      <c r="S182" s="10"/>
+      <c r="T182" s="10"/>
+      <c r="U182" s="10"/>
+      <c r="V182" s="10"/>
+      <c r="W182" s="10"/>
+      <c r="X182" s="10"/>
+      <c r="Y182" s="10"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="5" t="s">
@@ -4720,7 +4717,7 @@
         <v>21</v>
       </c>
       <c r="E183" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F183" s="5">
         <v>2.0</v>
@@ -4740,7 +4737,7 @@
         <v>21</v>
       </c>
       <c r="E184" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F184" s="5">
         <v>2.0</v>
@@ -4752,7 +4749,26 @@
         <v>48</v>
       </c>
     </row>
-    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1">
+      <c r="A185" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E185" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F185" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="G185" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="I185" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="186" ht="15.75" customHeight="1"/>
     <row r="187" ht="15.75" customHeight="1"/>
     <row r="188" ht="15.75" customHeight="1"/>
@@ -5538,6 +5554,7 @@
     <row r="968" ht="15.75" customHeight="1"/>
     <row r="969" ht="15.75" customHeight="1"/>
     <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="K1:N1"/>

</xml_diff>